<commit_message>
initial search functionality development / updated input for autocomplete / updated nearby activity to searchable select
</commit_message>
<xml_diff>
--- a/_documentation/API Design.xlsx
+++ b/_documentation/API Design.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\websites\adventure-properties\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\websites\adventure-properties\_documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088B77EE-8170-4FBB-A444-EE47B8112AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4037DEA-4866-473E-BFE7-4DFD86DC9354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CA46E04A-3417-4DD2-A052-9CC9E36FDA0B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>Resource</t>
   </si>
@@ -130,6 +130,15 @@
   </si>
   <si>
     <t>/properties/[propID]/reservations/users/userID</t>
+  </si>
+  <si>
+    <t>search for properties</t>
+  </si>
+  <si>
+    <t>/properties</t>
+  </si>
+  <si>
+    <t>Retrieve properties filtered by params</t>
   </si>
 </sst>
 </file>
@@ -527,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED28C55-32A6-4FA4-98BC-257CFD9FC3CE}">
-  <dimension ref="B2:O9"/>
+  <dimension ref="B2:O10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -597,11 +606,11 @@
         <v>17</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
@@ -610,51 +619,43 @@
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M5" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
     </row>
@@ -666,49 +667,53 @@
         <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
-        <v>10</v>
+    <row r="8" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -718,11 +723,36 @@
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>